<commit_message>
Recalculated all data points using new calibration curves (based on parsons gamma counter)
</commit_message>
<xml_diff>
--- a/Kocar_091316_BETAnalysis.xlsx
+++ b/Kocar_091316_BETAnalysis.xlsx
@@ -1,36 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27503"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kocar/Dropbox (MIT)/Ben/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="460" windowWidth="19200" windowHeight="11600"/>
+    <workbookView xWindow="1065" yWindow="465" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="BET Analysis" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
   <si>
     <t>BET Analysis Results</t>
   </si>
@@ -177,17 +174,24 @@
   </si>
   <si>
     <t>Sub-sampled</t>
+  </si>
+  <si>
+    <t>Mass sent</t>
+  </si>
+  <si>
+    <t>Calcualted SA from Mass Sent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000000"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -259,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -288,6 +292,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,22 +574,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45.5" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +598,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -599,7 +606,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -607,7 +614,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -642,7 +649,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
@@ -675,7 +682,7 @@
       </c>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
@@ -710,7 +717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>31</v>
       </c>
@@ -743,7 +750,7 @@
       </c>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>32</v>
       </c>
@@ -778,7 +785,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>33</v>
       </c>
@@ -811,7 +818,7 @@
       </c>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>34</v>
       </c>
@@ -846,7 +853,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>4</v>
       </c>
@@ -881,7 +888,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>5</v>
       </c>
@@ -916,7 +923,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>6</v>
       </c>
@@ -949,7 +956,7 @@
       </c>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>7</v>
       </c>
@@ -982,7 +989,7 @@
       </c>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>8</v>
       </c>
@@ -1017,7 +1024,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>36</v>
       </c>
@@ -1050,7 +1057,7 @@
       </c>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
@@ -1085,7 +1092,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>37</v>
       </c>
@@ -1118,7 +1125,7 @@
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>38</v>
       </c>
@@ -1152,8 +1159,14 @@
       <c r="K20" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>11</v>
       </c>
@@ -1185,8 +1198,15 @@
         <v>4.806</v>
       </c>
       <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21">
+        <v>0.1061</v>
+      </c>
+      <c r="M21" s="20">
+        <f>J21/L21</f>
+        <v>45.296889726672951</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>12</v>
       </c>
@@ -1218,8 +1238,15 @@
         <v>7.7759999999999998</v>
       </c>
       <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>0.19620000000000001</v>
+      </c>
+      <c r="M22" s="20">
+        <f>J22/L22</f>
+        <v>39.633027522935777</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>41</v>
       </c>
@@ -1251,8 +1278,15 @@
         <v>91.858000000000004</v>
       </c>
       <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>0.68010000000000004</v>
+      </c>
+      <c r="M23" s="21">
+        <f>J23/L23</f>
+        <v>135.06543155418322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>42</v>
       </c>
@@ -1286,8 +1320,12 @@
       <c r="K24" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M24" t="e">
+        <f>J24/L24</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>14</v>
       </c>
@@ -1319,8 +1357,15 @@
         <v>13.132999999999999</v>
       </c>
       <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="M25" s="21">
+        <f>J25/L25</f>
+        <v>196.89655172413794</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>39</v>
       </c>
@@ -1352,8 +1397,15 @@
         <v>0.52200000000000002</v>
       </c>
       <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26">
+        <v>8.8369999999999997</v>
+      </c>
+      <c r="M26" s="4">
+        <f>J26/L26</f>
+        <v>5.9069820074685982E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>40</v>
       </c>
@@ -1387,8 +1439,15 @@
       <c r="K27" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27">
+        <v>8.8369999999999997</v>
+      </c>
+      <c r="M27" s="4">
+        <f>J27/L27</f>
+        <v>7.8193957225302702E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C28" s="3"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1398,7 +1457,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C29" s="3"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -1408,7 +1467,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C30" s="3"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -1418,7 +1477,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C31" s="3"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1428,7 +1487,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C32" s="3"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1438,7 +1497,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1448,7 +1507,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1457,7 +1516,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" s="3"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1466,7 +1525,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C36" s="3"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1475,7 +1534,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="3"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1483,37 +1542,38 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="3"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="H38" s="6"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="H39" s="6"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final data changes, finalize igor pro figures
</commit_message>
<xml_diff>
--- a/Kocar_091316_BETAnalysis.xlsx
+++ b/Kocar_091316_BETAnalysis.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="465" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="1065" yWindow="465" windowWidth="19200" windowHeight="11595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BET Analysis" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -573,17 +573,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="45.42578125" customWidth="1"/>
@@ -1202,7 +1203,7 @@
         <v>0.1061</v>
       </c>
       <c r="M21" s="20">
-        <f>J21/L21</f>
+        <f t="shared" ref="M21:M27" si="0">J21/L21</f>
         <v>45.296889726672951</v>
       </c>
     </row>
@@ -1242,7 +1243,7 @@
         <v>0.19620000000000001</v>
       </c>
       <c r="M22" s="20">
-        <f>J22/L22</f>
+        <f t="shared" si="0"/>
         <v>39.633027522935777</v>
       </c>
     </row>
@@ -1282,7 +1283,7 @@
         <v>0.68010000000000004</v>
       </c>
       <c r="M23" s="21">
-        <f>J23/L23</f>
+        <f t="shared" si="0"/>
         <v>135.06543155418322</v>
       </c>
     </row>
@@ -1321,7 +1322,7 @@
         <v>44</v>
       </c>
       <c r="M24" t="e">
-        <f>J24/L24</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1361,7 +1362,7 @@
         <v>6.6699999999999995E-2</v>
       </c>
       <c r="M25" s="21">
-        <f>J25/L25</f>
+        <f t="shared" si="0"/>
         <v>196.89655172413794</v>
       </c>
     </row>
@@ -1401,7 +1402,7 @@
         <v>8.8369999999999997</v>
       </c>
       <c r="M26" s="4">
-        <f>J26/L26</f>
+        <f t="shared" si="0"/>
         <v>5.9069820074685982E-2</v>
       </c>
     </row>
@@ -1443,7 +1444,7 @@
         <v>8.8369999999999997</v>
       </c>
       <c r="M27" s="4">
-        <f>J27/L27</f>
+        <f t="shared" si="0"/>
         <v>7.8193957225302702E-2</v>
       </c>
     </row>
@@ -1458,118 +1459,118 @@
       <c r="J28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C33" s="3"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C34" s="3"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="6"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C35" s="3"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="6"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C36" s="3"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="6"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C37" s="3"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="H37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C38" s="3"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
       <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G38" s="6"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C39" s="3"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="H39" s="6"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C40" s="3"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C42" s="3"/>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C43" s="3"/>
     </row>
   </sheetData>

</xml_diff>